<commit_message>
adds CF attempt and p1 Dbfirst attempt
</commit_message>
<xml_diff>
--- a/p1reqs.xlsx
+++ b/p1reqs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Desktop\AllBatchFiles\ChristianRomeroP1\ChristianRomeroP1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{280B395D-831A-4745-A8B0-0043759E8942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E7D43D-CA38-413B-875F-5AC6D9052DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{713E5DAE-B2F3-4EE8-B899-4EA230B2DB04}"/>
+    <workbookView xWindow="1480" yWindow="1480" windowWidth="16920" windowHeight="10540" xr2:uid="{713E5DAE-B2F3-4EE8-B899-4EA230B2DB04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -249,12 +249,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -270,7 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -279,6 +303,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -599,7 +635,7 @@
   <dimension ref="A3:BI5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D5"/>
+      <selection activeCell="AR4" sqref="AR4:AR5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -794,15 +830,15 @@
         <v>61</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="6"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -810,62 +846,62 @@
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-      <c r="AC4" s="3"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="5"/>
       <c r="AD4" s="3"/>
-      <c r="AE4" s="3"/>
+      <c r="AE4" s="7"/>
       <c r="AF4" s="3"/>
       <c r="AG4" s="3"/>
-      <c r="AH4" s="3"/>
-      <c r="AI4" s="3"/>
-      <c r="AJ4" s="3"/>
+      <c r="AH4" s="5"/>
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="5"/>
       <c r="AK4" s="3"/>
-      <c r="AL4" s="3"/>
+      <c r="AL4" s="5"/>
       <c r="AM4" s="3"/>
       <c r="AN4" s="3"/>
       <c r="AO4" s="3"/>
       <c r="AP4" s="3"/>
       <c r="AQ4" s="3"/>
       <c r="AR4" s="3"/>
-      <c r="AS4" s="3"/>
+      <c r="AS4" s="7"/>
       <c r="AT4" s="3"/>
-      <c r="AU4" s="3"/>
-      <c r="AV4" s="3"/>
-      <c r="AW4" s="3"/>
-      <c r="AX4" s="3"/>
-      <c r="AY4" s="3"/>
+      <c r="AU4" s="7"/>
+      <c r="AV4" s="7"/>
+      <c r="AW4" s="7"/>
+      <c r="AX4" s="5"/>
+      <c r="AY4" s="7"/>
       <c r="AZ4" s="3"/>
-      <c r="BA4" s="3"/>
-      <c r="BB4" s="3"/>
-      <c r="BC4" s="3"/>
-      <c r="BD4" s="3"/>
-      <c r="BE4" s="3"/>
+      <c r="BA4" s="7"/>
+      <c r="BB4" s="5"/>
+      <c r="BC4" s="7"/>
+      <c r="BD4" s="7"/>
+      <c r="BE4" s="7"/>
       <c r="BF4" s="3"/>
-      <c r="BG4" s="3"/>
-      <c r="BH4" s="3"/>
-      <c r="BI4" s="3"/>
+      <c r="BG4" s="6"/>
+      <c r="BH4" s="6"/>
+      <c r="BI4" s="6"/>
     </row>
     <row r="5" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="6"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
@@ -873,49 +909,49 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="3"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="5"/>
       <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
+      <c r="AE5" s="7"/>
       <c r="AF5" s="3"/>
       <c r="AG5" s="3"/>
-      <c r="AH5" s="3"/>
-      <c r="AI5" s="3"/>
-      <c r="AJ5" s="3"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
       <c r="AK5" s="3"/>
-      <c r="AL5" s="3"/>
+      <c r="AL5" s="5"/>
       <c r="AM5" s="3"/>
       <c r="AN5" s="3"/>
       <c r="AO5" s="3"/>
       <c r="AP5" s="3"/>
       <c r="AQ5" s="3"/>
       <c r="AR5" s="3"/>
-      <c r="AS5" s="3"/>
+      <c r="AS5" s="7"/>
       <c r="AT5" s="3"/>
-      <c r="AU5" s="3"/>
-      <c r="AV5" s="3"/>
-      <c r="AW5" s="3"/>
-      <c r="AX5" s="3"/>
-      <c r="AY5" s="3"/>
+      <c r="AU5" s="7"/>
+      <c r="AV5" s="7"/>
+      <c r="AW5" s="7"/>
+      <c r="AX5" s="5"/>
+      <c r="AY5" s="7"/>
       <c r="AZ5" s="3"/>
-      <c r="BA5" s="3"/>
-      <c r="BB5" s="3"/>
-      <c r="BC5" s="3"/>
-      <c r="BD5" s="3"/>
-      <c r="BE5" s="3"/>
+      <c r="BA5" s="7"/>
+      <c r="BB5" s="5"/>
+      <c r="BC5" s="7"/>
+      <c r="BD5" s="7"/>
+      <c r="BE5" s="7"/>
       <c r="BF5" s="3"/>
-      <c r="BG5" s="3"/>
-      <c r="BH5" s="3"/>
-      <c r="BI5" s="3"/>
+      <c r="BG5" s="6"/>
+      <c r="BH5" s="6"/>
+      <c r="BI5" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="61">
@@ -929,11 +965,6 @@
     <mergeCell ref="BC4:BC5"/>
     <mergeCell ref="BD4:BD5"/>
     <mergeCell ref="BE4:BE5"/>
-    <mergeCell ref="AT4:AT5"/>
-    <mergeCell ref="AU4:AU5"/>
-    <mergeCell ref="AV4:AV5"/>
-    <mergeCell ref="AW4:AW5"/>
-    <mergeCell ref="AX4:AX5"/>
     <mergeCell ref="AY4:AY5"/>
     <mergeCell ref="AN4:AN5"/>
     <mergeCell ref="AO4:AO5"/>
@@ -941,11 +972,11 @@
     <mergeCell ref="AQ4:AQ5"/>
     <mergeCell ref="AR4:AR5"/>
     <mergeCell ref="AS4:AS5"/>
-    <mergeCell ref="AH4:AH5"/>
-    <mergeCell ref="AI4:AI5"/>
-    <mergeCell ref="AJ4:AJ5"/>
-    <mergeCell ref="AK4:AK5"/>
-    <mergeCell ref="AL4:AL5"/>
+    <mergeCell ref="AT4:AT5"/>
+    <mergeCell ref="AU4:AU5"/>
+    <mergeCell ref="AV4:AV5"/>
+    <mergeCell ref="AW4:AW5"/>
+    <mergeCell ref="AX4:AX5"/>
     <mergeCell ref="AM4:AM5"/>
     <mergeCell ref="AB4:AB5"/>
     <mergeCell ref="AC4:AC5"/>
@@ -953,11 +984,11 @@
     <mergeCell ref="AE4:AE5"/>
     <mergeCell ref="AF4:AF5"/>
     <mergeCell ref="AG4:AG5"/>
-    <mergeCell ref="V4:V5"/>
-    <mergeCell ref="W4:W5"/>
-    <mergeCell ref="X4:X5"/>
-    <mergeCell ref="Y4:Y5"/>
-    <mergeCell ref="Z4:Z5"/>
+    <mergeCell ref="AH4:AH5"/>
+    <mergeCell ref="AI4:AI5"/>
+    <mergeCell ref="AJ4:AJ5"/>
+    <mergeCell ref="AK4:AK5"/>
+    <mergeCell ref="AL4:AL5"/>
     <mergeCell ref="AA4:AA5"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
@@ -965,11 +996,11 @@
     <mergeCell ref="S4:S5"/>
     <mergeCell ref="T4:T5"/>
     <mergeCell ref="U4:U5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="V4:V5"/>
+    <mergeCell ref="W4:W5"/>
+    <mergeCell ref="X4:X5"/>
+    <mergeCell ref="Y4:Y5"/>
+    <mergeCell ref="Z4:Z5"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
@@ -980,6 +1011,11 @@
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Y3" r:id="rId1" location="core--domain--business-logic" display="https://github.com/06012021-dotnet-uta/06012021-dotnet-uta-batchrepo/wiki/Project-1-Requirements - core--domain--business-logic" xr:uid="{653A31F6-006D-4A34-B4D9-DE9FCCEA6198}"/>

</xml_diff>